<commit_message>
fix column rm_code in table report_members
</commit_message>
<xml_diff>
--- a/import/list_cntt_2.xlsx
+++ b/import/list_cntt_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\L A P T R I N H V I EN WEBSITE\Cd2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\L A P T R I N H V I EN WEBSITE\Cd2\nckh_ng\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC5FA07-2B3A-461A-9EBF-9E7410F8C39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18303295-8B32-477C-8946-8085980C43D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1011,13 +1011,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.21875" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>

</xml_diff>